<commit_message>
- Aider: envoi du Bonne Nouvelle de septembre (éd. 29.08.2013) - Aider: documentation mise à jour.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21357 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/2013-08-21.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/2013-08-21.xlsx
@@ -1362,12 +1362,6 @@
     <t>Ruchet</t>
   </si>
   <si>
-    <t>Route u Hameaux 9</t>
-  </si>
-  <si>
-    <t>Les Posses Bex</t>
-  </si>
-  <si>
     <t>Chevaney</t>
   </si>
   <si>
@@ -1951,6 +1945,12 @@
   </si>
   <si>
     <t>Grin-Vulliet</t>
+  </si>
+  <si>
+    <t>Les Posses-sur-Bex</t>
+  </si>
+  <si>
+    <t>Chalet la Ruche</t>
   </si>
 </sst>
 </file>
@@ -2411,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2429,28 +2429,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="8" t="s">
         <v>583</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>584</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2459,13 +2459,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>331</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="10">
@@ -2722,7 +2722,7 @@
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>45</v>
@@ -2791,7 +2791,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>56</v>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>59</v>
@@ -2863,7 +2863,7 @@
         <v>67</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="11">
@@ -3200,7 +3200,7 @@
         <v>1423</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3259,7 +3259,7 @@
         <v>129</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="11">
@@ -3649,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>185</v>
@@ -4018,7 +4018,7 @@
         <v>1000</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4033,7 +4033,7 @@
         <v>240</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="11">
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>242</v>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>244</v>
@@ -4096,7 +4096,7 @@
         <v>246</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>247</v>
@@ -4115,10 +4115,10 @@
         <v>2</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>249</v>
@@ -4282,7 +4282,7 @@
         <v>1337</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4311,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>277</v>
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>94</v>
@@ -4735,7 +4735,7 @@
         <v>335</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F105" s="6">
         <v>2156</v>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="B108" s="5"/>
       <c r="C108" s="4" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="4" t="s">
@@ -4821,20 +4821,20 @@
         <v>0</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>223</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F109" s="15"/>
       <c r="G109" s="11">
         <v>1844</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4884,7 +4884,7 @@
     <row r="112" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>352</v>
@@ -4909,13 +4909,13 @@
         <v>0</v>
       </c>
       <c r="C113" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="E113" s="4" t="s">
         <v>598</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="E113" s="4" t="s">
-        <v>600</v>
       </c>
       <c r="F113" s="15"/>
       <c r="G113" s="11">
@@ -4975,13 +4975,13 @@
         <v>0</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>362</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F116" s="15"/>
       <c r="G116" s="11">
@@ -5063,7 +5063,7 @@
         <v>0</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>373</v>
@@ -5076,7 +5076,7 @@
         <v>1426</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5113,7 +5113,7 @@
         <v>379</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F122" s="15"/>
       <c r="G122" s="11">
@@ -5129,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>380</v>
@@ -5157,7 +5157,7 @@
         <v>331</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F124" s="15"/>
       <c r="G124" s="11">
@@ -5208,7 +5208,7 @@
         <v>1304</v>
       </c>
       <c r="H126" s="4" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5423,14 +5423,14 @@
         <v>417</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F136" s="15"/>
       <c r="G136" s="11">
         <v>1054</v>
       </c>
       <c r="H136" s="4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5483,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>422</v>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>425</v>
@@ -5571,20 +5571,20 @@
         <v>0</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F143" s="15"/>
       <c r="G143" s="11">
         <v>1297</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5593,13 +5593,13 @@
         <v>0</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>210</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="F144" s="15"/>
       <c r="G144" s="11">
@@ -5687,14 +5687,14 @@
         <v>244</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>448</v>
+        <v>644</v>
       </c>
       <c r="F148" s="15"/>
       <c r="G148" s="11">
         <v>1880</v>
       </c>
       <c r="H148" s="4" t="s">
-        <v>449</v>
+        <v>643</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5703,20 +5703,20 @@
         <v>2</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F149" s="15"/>
       <c r="G149" s="11">
         <v>1071</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5725,20 +5725,20 @@
         <v>0</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>120</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F150" s="15"/>
       <c r="G150" s="11">
         <v>1085</v>
       </c>
       <c r="H150" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5747,13 +5747,13 @@
         <v>0</v>
       </c>
       <c r="C151" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="E151" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="D151" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>458</v>
       </c>
       <c r="F151" s="15"/>
       <c r="G151" s="11">
@@ -5769,13 +5769,13 @@
         <v>0</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D152" s="4" t="s">
         <v>331</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F152" s="15"/>
       <c r="G152" s="11">
@@ -5791,20 +5791,20 @@
         <v>2</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F153" s="15"/>
       <c r="G153" s="11">
         <v>1806</v>
       </c>
       <c r="H153" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5813,13 +5813,13 @@
         <v>0</v>
       </c>
       <c r="C154" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="E154" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="E154" s="4" t="s">
-        <v>466</v>
       </c>
       <c r="F154" s="15"/>
       <c r="G154" s="11">
@@ -5835,13 +5835,13 @@
         <v>0</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F155" s="15"/>
       <c r="G155" s="11">
@@ -5857,13 +5857,13 @@
         <v>0</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F156" s="15"/>
       <c r="G156" s="11">
@@ -5879,20 +5879,20 @@
         <v>0</v>
       </c>
       <c r="C157" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="E157" s="4" t="s">
         <v>471</v>
-      </c>
-      <c r="D157" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="E157" s="4" t="s">
-        <v>473</v>
       </c>
       <c r="F157" s="15"/>
       <c r="G157" s="11">
         <v>1803</v>
       </c>
       <c r="H157" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5901,20 +5901,20 @@
         <v>0</v>
       </c>
       <c r="C158" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="E158" s="4" t="s">
         <v>475</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>476</v>
-      </c>
-      <c r="E158" s="4" t="s">
-        <v>477</v>
       </c>
       <c r="F158" s="15"/>
       <c r="G158" s="11">
         <v>1885</v>
       </c>
       <c r="H158" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5923,13 +5923,13 @@
         <v>2</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>77</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F159" s="15"/>
       <c r="G159" s="11">
@@ -5945,20 +5945,20 @@
         <v>0</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>396</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F160" s="15"/>
       <c r="G160" s="11">
         <v>1317</v>
       </c>
       <c r="H160" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5967,13 +5967,13 @@
         <v>2</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>302</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F161" s="15"/>
       <c r="G161" s="11">
@@ -5989,20 +5989,20 @@
         <v>0</v>
       </c>
       <c r="C162" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="E162" s="4" t="s">
         <v>485</v>
-      </c>
-      <c r="D162" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="E162" s="4" t="s">
-        <v>487</v>
       </c>
       <c r="F162" s="15"/>
       <c r="G162" s="11">
         <v>1854</v>
       </c>
       <c r="H162" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6011,20 +6011,20 @@
         <v>0</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>168</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F163" s="15"/>
       <c r="G163" s="11">
         <v>1454</v>
       </c>
       <c r="H163" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6033,20 +6033,20 @@
         <v>2</v>
       </c>
       <c r="C164" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="E164" s="4" t="s">
         <v>492</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="E164" s="4" t="s">
-        <v>494</v>
       </c>
       <c r="F164" s="15"/>
       <c r="G164" s="11">
         <v>1522</v>
       </c>
       <c r="H164" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6055,13 +6055,13 @@
         <v>0</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F165" s="15"/>
       <c r="G165" s="11">
@@ -6077,13 +6077,13 @@
         <v>2</v>
       </c>
       <c r="C166" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="E166" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>500</v>
       </c>
       <c r="F166" s="15"/>
       <c r="G166" s="11">
@@ -6099,13 +6099,13 @@
         <v>2</v>
       </c>
       <c r="C167" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>501</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>503</v>
       </c>
       <c r="F167" s="15"/>
       <c r="G167" s="11">
@@ -6121,20 +6121,20 @@
         <v>0</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>144</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F168" s="15"/>
       <c r="G168" s="11">
         <v>1085</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6143,20 +6143,20 @@
         <v>2</v>
       </c>
       <c r="C169" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="E169" s="4" t="s">
         <v>506</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>508</v>
       </c>
       <c r="F169" s="15"/>
       <c r="G169" s="11">
         <v>1543</v>
       </c>
       <c r="H169" s="4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6171,14 +6171,14 @@
         <v>399</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F170" s="15"/>
       <c r="G170" s="11">
         <v>1607</v>
       </c>
       <c r="H170" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6187,20 +6187,20 @@
         <v>0</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>396</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F171" s="15"/>
       <c r="G171" s="11">
         <v>1131</v>
       </c>
       <c r="H171" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6209,13 +6209,13 @@
         <v>2</v>
       </c>
       <c r="C172" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="E172" s="4" t="s">
         <v>515</v>
-      </c>
-      <c r="D172" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="E172" s="4" t="s">
-        <v>517</v>
       </c>
       <c r="F172" s="15"/>
       <c r="G172" s="11">
@@ -6231,20 +6231,20 @@
         <v>0</v>
       </c>
       <c r="C173" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="E173" s="4" t="s">
         <v>518</v>
-      </c>
-      <c r="D173" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="E173" s="4" t="s">
-        <v>520</v>
       </c>
       <c r="F173" s="15"/>
       <c r="G173" s="11">
         <v>1274</v>
       </c>
       <c r="H173" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="174" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6253,13 +6253,13 @@
         <v>2</v>
       </c>
       <c r="C174" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E174" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="E174" s="4" t="s">
-        <v>524</v>
       </c>
       <c r="F174" s="15"/>
       <c r="G174" s="11">
@@ -6275,20 +6275,20 @@
         <v>0</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>214</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F175" s="15"/>
       <c r="G175" s="11">
         <v>1522</v>
       </c>
       <c r="H175" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="176" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6297,13 +6297,13 @@
         <v>0</v>
       </c>
       <c r="C176" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="E176" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="D176" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="E176" s="4" t="s">
-        <v>529</v>
       </c>
       <c r="F176" s="15"/>
       <c r="G176" s="11">
@@ -6319,20 +6319,20 @@
         <v>0</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>390</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F177" s="15"/>
       <c r="G177" s="11">
         <v>1515</v>
       </c>
       <c r="H177" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6341,20 +6341,20 @@
         <v>0</v>
       </c>
       <c r="C178" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="E178" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="D178" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="E178" s="4" t="s">
-        <v>535</v>
       </c>
       <c r="F178" s="15"/>
       <c r="G178" s="11">
         <v>1375</v>
       </c>
       <c r="H178" s="4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="179" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6363,20 +6363,20 @@
         <v>2</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F179" s="15"/>
       <c r="G179" s="11">
         <v>1071</v>
       </c>
       <c r="H179" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="180" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6385,13 +6385,13 @@
         <v>0</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>417</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F180" s="15"/>
       <c r="G180" s="11">
@@ -6407,13 +6407,13 @@
         <v>0</v>
       </c>
       <c r="C181" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="E181" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="D181" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="E181" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="F181" s="15"/>
       <c r="G181" s="11">
@@ -6432,10 +6432,10 @@
         <v>386</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E182" s="4" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F182" s="6">
         <v>104</v>
@@ -6444,7 +6444,7 @@
         <v>1522</v>
       </c>
       <c r="H182" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6453,20 +6453,20 @@
         <v>0</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>223</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F183" s="15"/>
       <c r="G183" s="11">
         <v>1526</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6481,7 +6481,7 @@
         <v>56</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F184" s="6">
         <v>63</v>
@@ -6490,7 +6490,7 @@
         <v>1522</v>
       </c>
       <c r="H184" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="185" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6499,20 +6499,20 @@
         <v>2</v>
       </c>
       <c r="C185" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E185" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="D185" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="E185" s="4" t="s">
-        <v>550</v>
       </c>
       <c r="F185" s="15"/>
       <c r="G185" s="11">
         <v>1522</v>
       </c>
       <c r="H185" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6521,13 +6521,13 @@
         <v>0</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D186" s="4" t="s">
         <v>362</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="F186" s="6">
         <v>827</v>
@@ -6536,7 +6536,7 @@
         <v>1885</v>
       </c>
       <c r="H186" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6545,13 +6545,13 @@
         <v>0</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D187" s="4" t="s">
         <v>417</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F187" s="15"/>
       <c r="G187" s="11">
@@ -6567,20 +6567,20 @@
         <v>2</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D188" s="4" t="s">
         <v>302</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F188" s="15"/>
       <c r="G188" s="11">
         <v>1820</v>
       </c>
       <c r="H188" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6589,13 +6589,13 @@
         <v>0</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D189" s="4" t="s">
         <v>120</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F189" s="15"/>
       <c r="G189" s="11">
@@ -6611,20 +6611,20 @@
         <v>2</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D190" s="4" t="s">
         <v>335</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F190" s="15"/>
       <c r="G190" s="11">
         <v>1278</v>
       </c>
       <c r="H190" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="191" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6633,13 +6633,13 @@
         <v>0</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D191" s="4" t="s">
         <v>414</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F191" s="15"/>
       <c r="G191" s="11">
@@ -6661,7 +6661,7 @@
         <v>12</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F192" s="15"/>
       <c r="G192" s="11">
@@ -6677,13 +6677,13 @@
         <v>2</v>
       </c>
       <c r="C193" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="E193" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="E193" s="4" t="s">
-        <v>567</v>
       </c>
       <c r="F193" s="15"/>
       <c r="G193" s="11">
@@ -6699,20 +6699,20 @@
         <v>0</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F194" s="15"/>
       <c r="G194" s="11">
         <v>1880</v>
       </c>
       <c r="H194" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="195" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6743,13 +6743,13 @@
         <v>2</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D196" s="4" t="s">
         <v>376</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F196" s="15"/>
       <c r="G196" s="11">
@@ -6765,20 +6765,20 @@
         <v>0</v>
       </c>
       <c r="C197" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="E197" s="4" t="s">
         <v>572</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>574</v>
       </c>
       <c r="F197" s="15"/>
       <c r="G197" s="11">
         <v>1522</v>
       </c>
       <c r="H197" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6787,20 +6787,20 @@
         <v>0</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D198" s="4" t="s">
         <v>132</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F198" s="15"/>
       <c r="G198" s="11">
         <v>1041</v>
       </c>
       <c r="H198" s="4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6809,20 +6809,20 @@
         <v>2</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F199" s="15"/>
       <c r="G199" s="11">
         <v>1041</v>
       </c>
       <c r="H199" s="4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6837,14 +6837,14 @@
         <v>223</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F200" s="15"/>
       <c r="G200" s="11">
         <v>1058</v>
       </c>
       <c r="H200" s="4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>